<commit_message>
added more lights. added functionality to resize or hide foundation base on finished construction.
Former-commit-id: 89b806be7f6c3fda6363b69916668d19f4257035 [formerly d024b349f68d5909d7fe53998fff9040585ad2b6]
Former-commit-id: 0601910596cbd40add98b00dc961a35d8a72b6e0
</commit_message>
<xml_diff>
--- a/NewCaldera/NewCaldera.AssetBundles/Assets/Locales/Outward-Lights/English/Outward-Lights_BuildingLocales_English.xlsx
+++ b/NewCaldera/NewCaldera.AssetBundles/Assets/Locales/Outward-Lights/English/Outward-Lights_BuildingLocales_English.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\modifamorphic\GitHub-Outward\mods\newcaldera\outward\NewCaldera\NewCaldera.AssetBundles\Assets\Locales\NewSirocco-Lights\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\modifamorphic\GitHub-Outward\mods\newcaldera\outward\NewCaldera\NewCaldera.AssetBundles\Assets\Locales\Outward-Lights\English\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D179EAF5-0F4A-4040-B1D2-F00A0587C604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91014E84-6043-4A13-B19D-43ECA21F9F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10420" yWindow="3700" windowWidth="24170" windowHeight="15580" xr2:uid="{080F41EB-CBDA-473A-A4F4-758392FABC81}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{080F41EB-CBDA-473A-A4F4-758392FABC81}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingLocales_English" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>ItemID</t>
   </si>
@@ -42,23 +42,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Levant style floor lantern.
-----
-Construction requirements
-  Funds: {funds_cost}
-  Food: {food_cost}
-  Stone: {stone_cost}
-  Material:  {item1_cost}
-  Funds upkeep: {funds_upkeep} / Day
-Construction:  {build_days} Days</t>
-  </si>
-  <si>
-    <t>Blueprint: Light - Levant Lantern</t>
-  </si>
-  <si>
-    <t>- Levant Lantern</t>
   </si>
   <si>
     <t>- Harmattan Lamp Post</t>
@@ -85,6 +68,91 @@
   </si>
   <si>
     <t>A raging bonfire.
+----
+Construction requirements
+  Funds: {funds_cost}
+  Food: {food_cost}
+  Stone: {stone_cost}
+  Material:  {item1_cost}
+  Funds upkeep: {funds_upkeep} / Day
+Construction:  {build_days} Days</t>
+  </si>
+  <si>
+    <t>Blueprint: Light - Stone Lantern</t>
+  </si>
+  <si>
+    <t>Blueprint: Light - Stylish Floor Lamp</t>
+  </si>
+  <si>
+    <t>-  Stylish Floor Lamp</t>
+  </si>
+  <si>
+    <t>Stylish floor lamp common to the Berg and Levant regions.
+----
+Construction requirements
+  Funds: {funds_cost}
+  Food: {food_cost}
+  Stone: {stone_cost}
+  Material:  {item1_cost}
+  Funds upkeep: {funds_upkeep} / Day
+Construction:  {build_days} Days</t>
+  </si>
+  <si>
+    <t>- Stone Lantern</t>
+  </si>
+  <si>
+    <t>Stone floor lantern.
+----
+Construction requirements
+  Funds: {funds_cost}
+  Food: {food_cost}
+  Stone: {stone_cost}
+  Material:  {item1_cost}
+  Funds upkeep: {funds_upkeep} / Day
+Construction:  {build_days} Days</t>
+  </si>
+  <si>
+    <t>Blueprint: Light - Barrel Lamp</t>
+  </si>
+  <si>
+    <t>- Barrel Lamp</t>
+  </si>
+  <si>
+    <t>Barrel shaped floor lamp.
+----
+Construction requirements
+  Funds: {funds_cost}
+  Food: {food_cost}
+  Stone: {stone_cost}
+  Material:  {item1_cost}
+  Funds upkeep: {funds_upkeep} / Day
+Construction:  {build_days} Days</t>
+  </si>
+  <si>
+    <t>- Cold Stone Lantern</t>
+  </si>
+  <si>
+    <t>Blueprint: Light - Cold Stone Lantern</t>
+  </si>
+  <si>
+    <t>Cold Stone floor lantern.
+----
+Construction requirements
+  Funds: {funds_cost}
+  Food: {food_cost}
+  Stone: {stone_cost}
+  Material:  {item1_cost}
+  Funds upkeep: {funds_upkeep} / Day
+Construction:  {build_days} Days</t>
+  </si>
+  <si>
+    <t>Blueprint: Light - Stone Sun Pillar</t>
+  </si>
+  <si>
+    <t>- Stone Sun Pillar</t>
+  </si>
+  <si>
+    <t>Large stone sun pillar waypoint.
 ----
 Construction requirements
   Funds: {funds_cost}
@@ -449,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D412611E-C54F-46D1-9616-C965D11EFD52}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -478,10 +546,10 @@
         <v>-1330060100</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -489,7 +557,7 @@
         <v>-1330060101</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
@@ -497,10 +565,10 @@
         <v>-1330060110</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -508,7 +576,7 @@
         <v>-1330060111</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
@@ -516,10 +584,10 @@
         <v>-1330060120</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -527,7 +595,83 @@
         <v>-1330060121</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>-1330060130</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>-1330060131</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>-1330060140</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>-1330060141</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>-1330060150</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>-1330060151</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>-1330060200</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>-1330060201</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>